<commit_message>
Salva as predições do PCR (em dados com MSC) no formato XLSX
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_msc.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_msc.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7628381098970708</v>
+        <v>0.7628380883927329</v>
       </c>
       <c r="D2" t="n">
-        <v>3.319182292800534</v>
+        <v>3.319182593762956</v>
       </c>
       <c r="E2" t="n">
-        <v>1.293645143472821</v>
+        <v>1.293645202122592</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7628381098970709</v>
+        <v>0.7628380883927335</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7532931155593524</v>
+        <v>0.7532930963252453</v>
       </c>
       <c r="D3" t="n">
-        <v>3.462314329291304</v>
+        <v>3.462314590300782</v>
       </c>
       <c r="E3" t="n">
-        <v>1.384472971641167</v>
+        <v>1.384473021753507</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7283663675710513</v>
+        <v>0.7283663479069661</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4196208516565313</v>
+        <v>0.41962086079582</v>
       </c>
       <c r="D4" t="n">
-        <v>1.90626692031709</v>
+        <v>1.906266890298914</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2349628777210636</v>
+        <v>0.2349628758710716</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4196208516565312</v>
+        <v>0.4196208607958198</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3832151630337233</v>
+        <v>0.383215171516247</v>
       </c>
       <c r="D5" t="n">
-        <v>2.025054734055889</v>
+        <v>2.025054706100264</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2511248865545974</v>
+        <v>0.2511248847312456</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3370316392274644</v>
+        <v>0.3370316488547423</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4794205967897539</v>
+        <v>0.4794205967898998</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5844946549666763</v>
+        <v>0.5844946549665129</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4231102784328025</v>
+        <v>0.4231102784327432</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4794205967897537</v>
+        <v>0.4794205967898995</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4605094946514083</v>
+        <v>0.4605094946515488</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6056666490331792</v>
+        <v>0.6056666490330206</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4413826298146344</v>
+        <v>0.4413826298145789</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4334864447869325</v>
+        <v>0.433486444787075</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5301974113372021</v>
+        <v>0.5301974560736974</v>
       </c>
       <c r="D8" t="n">
-        <v>241.0134689632815</v>
+        <v>241.0134460130078</v>
       </c>
       <c r="E8" t="n">
-        <v>70.44077089442879</v>
+        <v>70.44076754060168</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5301974113372017</v>
+        <v>0.5301974560736973</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4985126820411977</v>
+        <v>0.4985127294126936</v>
       </c>
       <c r="D9" t="n">
-        <v>257.0147952601153</v>
+        <v>257.0147716569624</v>
       </c>
       <c r="E9" t="n">
-        <v>76.11309739514756</v>
+        <v>76.11309352548025</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4514881725568465</v>
+        <v>0.4514882283306437</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6739385547807242</v>
+        <v>0.6739385443537061</v>
       </c>
       <c r="D10" t="n">
-        <v>5.001468216432992</v>
+        <v>5.001468376373388</v>
       </c>
       <c r="E10" t="n">
-        <v>1.836866562504975</v>
+        <v>1.836866591875267</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6739385547807243</v>
+        <v>0.6739385443537067</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.652690478143148</v>
+        <v>0.6526904664109401</v>
       </c>
       <c r="D11" t="n">
-        <v>5.33409356768285</v>
+        <v>5.334093756197418</v>
       </c>
       <c r="E11" t="n">
-        <v>1.987495001907254</v>
+        <v>1.987495021437214</v>
       </c>
       <c r="F11" t="n">
-        <v>0.618269973490281</v>
+        <v>0.6182699659882021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Salva as predições do PCR em dados com Multiplicative Scatter Correction
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_msc.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_msc.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7628380883927329</v>
+        <v>0.7628380416766974</v>
       </c>
       <c r="D2" t="n">
-        <v>3.319182593762956</v>
+        <v>3.319183247573894</v>
       </c>
       <c r="E2" t="n">
-        <v>1.293645202122592</v>
+        <v>1.29364532953338</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7628380883927335</v>
+        <v>0.7628380416766979</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7532930963252453</v>
+        <v>0.7532930426306966</v>
       </c>
       <c r="D3" t="n">
-        <v>3.462314590300782</v>
+        <v>3.462315349976672</v>
       </c>
       <c r="E3" t="n">
-        <v>1.384473021753507</v>
+        <v>1.384473141169541</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7283663479069661</v>
+        <v>0.7283663010481045</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.41962086079582</v>
+        <v>0.4196208449933275</v>
       </c>
       <c r="D4" t="n">
-        <v>1.906266890298914</v>
+        <v>1.906266942202516</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2349628758710716</v>
+        <v>0.2349628790698418</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4196208607958198</v>
+        <v>0.4196208449933276</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.383215171516247</v>
+        <v>0.3832151557809966</v>
       </c>
       <c r="D5" t="n">
-        <v>2.025054706100264</v>
+        <v>2.025054757843534</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2511248847312456</v>
+        <v>0.2511248879780174</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3370316488547423</v>
+        <v>0.3370316317118217</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4794205967898998</v>
+        <v>0.4794205967899169</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5844946549665129</v>
+        <v>0.5844946549664933</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4231102784327432</v>
+        <v>0.4231102784327361</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4794205967898995</v>
+        <v>0.4794205967899169</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4605094946515488</v>
+        <v>0.4605094946515672</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6056666490330206</v>
+        <v>0.6056666490330013</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4413826298145789</v>
+        <v>0.4413826298145707</v>
       </c>
       <c r="F7" t="n">
-        <v>0.433486444787075</v>
+        <v>0.433486444787096</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5301974560736974</v>
+        <v>0.5301972677079847</v>
       </c>
       <c r="D8" t="n">
-        <v>241.0134460130078</v>
+        <v>241.0135426465194</v>
       </c>
       <c r="E8" t="n">
-        <v>70.44076754060168</v>
+        <v>70.44078166209192</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5301974560736973</v>
+        <v>0.5301972677079844</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4985127294126936</v>
+        <v>0.4985125194928611</v>
       </c>
       <c r="D9" t="n">
-        <v>257.0147716569624</v>
+        <v>257.014877413188</v>
       </c>
       <c r="E9" t="n">
-        <v>76.11309352548025</v>
+        <v>76.11311164301578</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4514882283306437</v>
+        <v>0.4514879672012574</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6739385443537061</v>
+        <v>0.6739385215215666</v>
       </c>
       <c r="D10" t="n">
-        <v>5.001468376373388</v>
+        <v>5.001468726596397</v>
       </c>
       <c r="E10" t="n">
-        <v>1.836866591875267</v>
+        <v>1.836866656187675</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6739385443537067</v>
+        <v>0.6739385215215666</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6526904664109401</v>
+        <v>0.6526904401543469</v>
       </c>
       <c r="D11" t="n">
-        <v>5.334093756197418</v>
+        <v>5.334094156053612</v>
       </c>
       <c r="E11" t="n">
-        <v>1.987495021437214</v>
+        <v>1.987495126038354</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6182699659882021</v>
+        <v>0.6182699258075751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adiciona arquivos com informações do plot do PCR com filtro MSC
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_msc.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_msc.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7628380416766974</v>
+        <v>0.7066831166592121</v>
       </c>
       <c r="D2" t="n">
-        <v>3.319183247573894</v>
+        <v>4.105095489590036</v>
       </c>
       <c r="E2" t="n">
-        <v>1.29364532953338</v>
+        <v>1.43867018000876</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7628380416766979</v>
+        <v>0.7066831166592127</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.7532930426306966</v>
+        <v>0.6971472239506631</v>
       </c>
       <c r="D3" t="n">
-        <v>3.462315349976672</v>
+        <v>4.248792685760669</v>
       </c>
       <c r="E3" t="n">
-        <v>1.384473141169541</v>
+        <v>1.501580499894976</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7283663010481045</v>
+        <v>0.6804698690085806</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4196208449933275</v>
+        <v>0.4246018788223884</v>
       </c>
       <c r="D4" t="n">
-        <v>1.906266942202516</v>
+        <v>1.889906636970288</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2349628790698418</v>
+        <v>0.233952436166282</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4196208449933276</v>
+        <v>0.4246018788223885</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3832151557809966</v>
+        <v>0.3770829766081768</v>
       </c>
       <c r="D5" t="n">
-        <v>2.025054757843534</v>
+        <v>2.045259850466442</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2511248879780174</v>
+        <v>0.2547892213537854</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3370316317118217</v>
+        <v>0.317542833205385</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.4794205967899169</v>
+        <v>0.4907501243415704</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5844946549664933</v>
+        <v>0.571774120392127</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4231102784327361</v>
+        <v>0.4184808130584473</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4794205967899169</v>
+        <v>0.4907501243415697</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4605094946515672</v>
+        <v>0.4689316096842102</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6056666490330013</v>
+        <v>0.5957137074257653</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4413826298145707</v>
+        <v>0.439661175291062</v>
       </c>
       <c r="F7" t="n">
-        <v>0.433486444787096</v>
+        <v>0.4378967930628836</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5301972677079847</v>
+        <v>0.4688519577727558</v>
       </c>
       <c r="D8" t="n">
-        <v>241.0135426465194</v>
+        <v>272.4843057051052</v>
       </c>
       <c r="E8" t="n">
-        <v>70.44078166209192</v>
+        <v>74.89868450622626</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5301972677079844</v>
+        <v>0.4688519577727559</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4985125194928611</v>
+        <v>0.4496581277214421</v>
       </c>
       <c r="D9" t="n">
-        <v>257.014877413188</v>
+        <v>282.0857255247623</v>
       </c>
       <c r="E9" t="n">
-        <v>76.11311164301578</v>
+        <v>77.72414758689595</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4514879672012574</v>
+        <v>0.4280222426172862</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6739385215215666</v>
+        <v>0.6324113483372988</v>
       </c>
       <c r="D10" t="n">
-        <v>5.001468726596397</v>
+        <v>5.638455527227638</v>
       </c>
       <c r="E10" t="n">
-        <v>1.836866656187675</v>
+        <v>1.95033372924551</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6739385215215666</v>
+        <v>0.6324113483372984</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6526904401543469</v>
+        <v>0.6172330804647074</v>
       </c>
       <c r="D11" t="n">
-        <v>5.334094156053612</v>
+        <v>5.878397254636925</v>
       </c>
       <c r="E11" t="n">
-        <v>1.987495126038354</v>
+        <v>2.047961053186884</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6182699258075751</v>
+        <v>0.5946897203806566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza legenda na plotagem dos gráficos do PCR
</commit_message>
<xml_diff>
--- a/Partial Components Regression/plot_infos_pcr_msc.xlsx
+++ b/Partial Components Regression/plot_infos_pcr_msc.xlsx
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7066831166592163</v>
+        <v>0.7066831166572116</v>
       </c>
       <c r="D2" t="n">
-        <v>1.438670180008751</v>
+        <v>1.438670180013667</v>
       </c>
       <c r="E2" t="n">
-        <v>4.105095489589983</v>
+        <v>4.10509548961804</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7066831166592163</v>
+        <v>0.7066831166572113</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6804698690085335</v>
+        <v>0.6804698690063254</v>
       </c>
       <c r="D3" t="n">
-        <v>1.501580499895086</v>
+        <v>1.501580499900274</v>
       </c>
       <c r="E3" t="n">
-        <v>4.248792685759586</v>
+        <v>4.248792685800696</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6971472239507518</v>
+        <v>0.6971472239479968</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.582392765366923</v>
+        <v>0.5823927653686751</v>
       </c>
       <c r="D4" t="n">
-        <v>1.359874398235301</v>
+        <v>1.359874398232449</v>
       </c>
       <c r="E4" t="n">
-        <v>1.764861058949153</v>
+        <v>1.764861058943934</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8890481639202232</v>
+        <v>0.8890481639222548</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.4246018486687569</v>
+        <v>0.4246018430476296</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2339524422963989</v>
+        <v>0.2339524434391524</v>
       </c>
       <c r="E5" t="n">
-        <v>1.889906736010495</v>
+        <v>1.889906754473197</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4246018486687571</v>
+        <v>0.4246018430476307</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3175427648022607</v>
+        <v>0.3175427740650335</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2547892341226295</v>
+        <v>0.2547892323935432</v>
       </c>
       <c r="E6" t="n">
-        <v>2.04525999503011</v>
+        <v>2.045259981327476</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3770829326099566</v>
+        <v>0.3770829371141529</v>
       </c>
     </row>
     <row r="7">
@@ -597,16 +597,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.4193890325460984</v>
+        <v>0.4193889020671729</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2008072895261398</v>
+        <v>0.2008073120895423</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6091880822025666</v>
+        <v>0.6091880904684288</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8234431080378893</v>
+        <v>0.8234431210451721</v>
       </c>
     </row>
     <row r="8">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4907501243441826</v>
+        <v>0.4907501243438135</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4184808130573737</v>
+        <v>0.4184808130575254</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5717741203891936</v>
+        <v>0.5717741203896081</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4907501243441822</v>
+        <v>0.4907501243438137</v>
       </c>
     </row>
     <row r="9">
@@ -645,16 +645,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4378967930685279</v>
+        <v>0.4378967930686819</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4396611752888547</v>
+        <v>0.4396611752887944</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5957137074218271</v>
+        <v>0.5957137074221712</v>
       </c>
       <c r="F9" t="n">
-        <v>0.468931609688125</v>
+        <v>0.4689316096879387</v>
       </c>
     </row>
     <row r="10">
@@ -669,16 +669,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.4715904908622609</v>
+        <v>0.471590490861763</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3179403569792187</v>
+        <v>0.3179403569793685</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.01515743881380183</v>
+        <v>-0.01515743881349407</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9513338876576261</v>
+        <v>0.9513338876561829</v>
       </c>
     </row>
     <row r="11">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.468851957774996</v>
+        <v>0.4688519577738969</v>
       </c>
       <c r="D11" t="n">
-        <v>74.89868450606831</v>
+        <v>74.89868450614581</v>
       </c>
       <c r="E11" t="n">
-        <v>272.4843057039558</v>
+        <v>272.4843057045198</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4688519577749965</v>
+        <v>0.4688519577738967</v>
       </c>
     </row>
     <row r="12">
@@ -717,16 +717,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.4280222426197769</v>
+        <v>0.4280222426185856</v>
       </c>
       <c r="D12" t="n">
-        <v>77.72414758672673</v>
+        <v>77.72414758680766</v>
       </c>
       <c r="E12" t="n">
-        <v>282.0857255236262</v>
+        <v>282.0857255241843</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4496581277236957</v>
+        <v>0.4496581277225765</v>
       </c>
     </row>
     <row r="13">
@@ -741,16 +741,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.4698552868879904</v>
+        <v>0.4698552868867564</v>
       </c>
       <c r="D13" t="n">
-        <v>56.25050462134656</v>
+        <v>56.25050462141203</v>
       </c>
       <c r="E13" t="n">
-        <v>3.660049469787396</v>
+        <v>3.660049470391812</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9676263846128885</v>
+        <v>0.9676263846116978</v>
       </c>
     </row>
     <row r="14">
@@ -765,16 +765,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.6324113483372676</v>
+        <v>0.6324113483373592</v>
       </c>
       <c r="D14" t="n">
-        <v>1.950333729245592</v>
+        <v>1.950333729245349</v>
       </c>
       <c r="E14" t="n">
-        <v>5.638455527228118</v>
+        <v>5.638455527226712</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6324113483372673</v>
+        <v>0.632411348337359</v>
       </c>
     </row>
     <row r="15">
@@ -789,16 +789,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.5946897203807606</v>
+        <v>0.594689720380671</v>
       </c>
       <c r="D15" t="n">
-        <v>2.047961053186621</v>
+        <v>2.047961053186847</v>
       </c>
       <c r="E15" t="n">
-        <v>5.878397254636665</v>
+        <v>5.878397254636694</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6172330804647264</v>
+        <v>0.6172330804647287</v>
       </c>
     </row>
     <row r="16">
@@ -813,16 +813,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.6326836387267732</v>
+        <v>0.6326836387264478</v>
       </c>
       <c r="D16" t="n">
-        <v>1.313405097363099</v>
+        <v>1.313405097363681</v>
       </c>
       <c r="E16" t="n">
-        <v>2.841349805743501</v>
+        <v>2.841349805747715</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8253233738178234</v>
+        <v>0.8253233738172396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>